<commit_message>
updates project metadata and metadata table names
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Downloads/metadata template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C65B6D1-F120-C24B-9F61-6C154BA6B93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F07A8F-3F58-6448-B524-1F6B1810F5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="25520" windowHeight="15280" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="25520" windowHeight="15280" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>first_name</t>
   </si>
@@ -166,13 +166,88 @@
   </si>
   <si>
     <t xml:space="preserve">geometry </t>
+  </si>
+  <si>
+    <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>2023-01-05</t>
+  </si>
+  <si>
+    <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on  Battle Creek and Clear Creek</t>
+  </si>
+  <si>
+    <t>tabular</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Wingerter</t>
+  </si>
+  <si>
+    <t>natasha_wingerter@fws.gov</t>
+  </si>
+  <si>
+    <t>USFWS</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Battle and Clear Creek RST</t>
+  </si>
+  <si>
+    <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on Battle and Clear Creek</t>
+  </si>
+  <si>
+    <t>spring run</t>
+  </si>
+  <si>
+    <t>fall run</t>
+  </si>
+  <si>
+    <t>trap</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>juvenile production estimate</t>
+  </si>
+  <si>
+    <t>Oncorhynchus tshawytscha</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Central Valley</t>
+  </si>
+  <si>
+    <t>CCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ongoing </t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>Battle and Clear Creek RST program</t>
+  </si>
+  <si>
+    <t>chinook</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -201,6 +276,24 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -236,17 +329,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -258,6 +347,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -345,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -633,7 +729,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,16 +737,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC88997-D746-4692-9A7F-1A0E218D4835}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9"/>
+    <col min="3" max="3" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -660,17 +756,28 @@
       <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{1233EF59-08AA-402F-97DC-7F1A6FD6CFFE}">
       <formula1>" Point, LineString, LinearRing, Polygon, Multipoint, MultiLineString, MultiPolygon, MultiGeometry"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{0D49A741-B9FC-40CC-92FB-9400626C24F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3:B1048576" xr:uid="{0D49A741-B9FC-40CC-92FB-9400626C24F0}">
       <formula1>"tabular, vector, raster"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2" xr:uid="{C6C6262D-2579-E149-9D0F-C026F9C95328}">
+      <formula1>"tabular,vector,raster"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -679,52 +786,57 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="8" width="10.5" style="9"/>
-    <col min="9" max="9" width="10.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21" style="7" customWidth="1"/>
+    <col min="4" max="8" width="10.5" style="7"/>
+    <col min="9" max="9" width="10.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -743,14 +855,14 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27" style="7" customWidth="1"/>
+    <col min="6" max="6" width="27" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -769,13 +881,26 @@
       <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
-      <c r="E2" s="2"/>
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
@@ -788,6 +913,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:natasha_wingerter@fws.gov" xr:uid="{F26F2F54-C5D1-7F46-8A28-EBB5CCE07E19}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -798,7 +926,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,7 +944,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -826,27 +959,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -855,36 +1032,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="9"/>
-    <col min="4" max="4" width="15.1640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="7"/>
+    <col min="4" max="4" width="15.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="26" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -900,39 +1082,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9" style="9"/>
-    <col min="3" max="3" width="9" style="7"/>
-    <col min="4" max="4" width="9" style="9"/>
-    <col min="5" max="5" width="14.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9" style="7"/>
+    <col min="1" max="2" width="9" style="7"/>
+    <col min="3" max="3" width="9" style="5"/>
+    <col min="4" max="4" width="9" style="7"/>
+    <col min="5" max="5" width="14.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -942,6 +1141,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:natasha_wingerter@fws.gov" xr:uid="{C9B4ACE4-4B13-A344-A5FA-21E01A84058F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -957,40 +1159,40 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="7"/>
-    <col min="6" max="6" width="17.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5"/>
+    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1005,23 +1207,31 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1044,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1270,7 @@
     <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1083,33 +1293,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G8" s="6"/>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G8 G3" xr:uid="{D0FABE90-94BB-4510-8A04-3DED000903A4}">
-      <formula1>F2</formula1>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G8" xr:uid="{D0FABE90-94BB-4510-8A04-3DED000903A4}">
+      <formula1>F3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
validates xml with updates to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F07A8F-3F58-6448-B524-1F6B1810F5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE92E5-2471-4A4C-9BB6-78FD5E5D6761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="25520" windowHeight="15280" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>first_name</t>
   </si>
@@ -168,39 +168,45 @@
     <t xml:space="preserve">geometry </t>
   </si>
   <si>
-    <t>2020-07-06</t>
-  </si>
-  <si>
-    <t>2023-01-05</t>
-  </si>
-  <si>
-    <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on  Battle Creek and Clear Creek</t>
+    <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on  Battle and Clear Creek</t>
   </si>
   <si>
     <t>tabular</t>
   </si>
   <si>
+    <t>natasha_wingerter@fws.gov</t>
+  </si>
+  <si>
     <t>Natasha</t>
   </si>
   <si>
     <t>Wingerter</t>
   </si>
   <si>
-    <t>natasha_wingerter@fws.gov</t>
-  </si>
-  <si>
-    <t>USFWS</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
-    <t>Battle and Clear Creek RST</t>
+    <t>U.S. Fish and Wildlife Service</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schraml </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mike_schraml@fws.gov </t>
+  </si>
+  <si>
+    <t>principal investigator</t>
   </si>
   <si>
     <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on Battle and Clear Creek</t>
   </si>
   <si>
+    <t>Battle and Clear RST</t>
+  </si>
+  <si>
     <t>spring run</t>
   </si>
   <si>
@@ -228,7 +234,7 @@
     <t>Central Valley</t>
   </si>
   <si>
-    <t>CCO</t>
+    <t>CCBY</t>
   </si>
   <si>
     <t xml:space="preserve">ongoing </t>
@@ -237,17 +243,21 @@
     <t>monthly</t>
   </si>
   <si>
-    <t>Battle and Clear Creek RST program</t>
-  </si>
-  <si>
     <t>chinook</t>
+  </si>
+  <si>
+    <t>Battle and Clear Rotary Screw Traps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -264,13 +274,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF494A4C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -279,20 +282,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -329,11 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -347,13 +346,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -740,12 +744,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -761,23 +765,20 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>47</v>
+      <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{1233EF59-08AA-402F-97DC-7F1A6FD6CFFE}">
       <formula1>" Point, LineString, LinearRing, Polygon, Multipoint, MultiLineString, MultiPolygon, MultiGeometry"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3:B1048576" xr:uid="{0D49A741-B9FC-40CC-92FB-9400626C24F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{0D49A741-B9FC-40CC-92FB-9400626C24F0}">
       <formula1>"tabular, vector, raster"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2" xr:uid="{C6C6262D-2579-E149-9D0F-C026F9C95328}">
-      <formula1>"tabular,vector,raster"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -788,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +837,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -855,7 +856,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,24 +888,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -914,7 +928,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:natasha_wingerter@fws.gov" xr:uid="{F26F2F54-C5D1-7F46-8A28-EBB5CCE07E19}"/>
+    <hyperlink ref="C3" r:id="rId1" display="mailto:mike_schraml@fws.gov" xr:uid="{F2D40BA9-AE88-344B-8932-8A4AF3E71FFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -926,7 +940,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,11 +958,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
+      <c r="A2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -980,48 +994,48 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>55</v>
+      <c r="A2" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>56</v>
+      <c r="A3" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>57</v>
+      <c r="A4" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>58</v>
+      <c r="A5" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>59</v>
+      <c r="A6" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>60</v>
+      <c r="A7" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>61</v>
+      <c r="A8" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>62</v>
+      <c r="A9" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>63</v>
+      <c r="A10" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1080,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1118,20 +1132,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1141,9 +1155,6 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:natasha_wingerter@fws.gov" xr:uid="{C9B4ACE4-4B13-A344-A5FA-21E01A84058F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1187,10 +1198,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
@@ -1228,10 +1239,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1254,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1281,7 @@
     <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1293,46 +1304,55 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>-122.49641099999999</v>
+      </c>
+      <c r="C2">
+        <v>-121.75038600000001</v>
+      </c>
+      <c r="D2">
+        <v>40.505833330000002</v>
+      </c>
+      <c r="E2">
+        <v>39.622342000000003</v>
+      </c>
+      <c r="F2" s="16">
+        <v>43831</v>
+      </c>
+      <c r="G2" s="16">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G8" xr:uid="{D0FABE90-94BB-4510-8A04-3DED000903A4}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G8" xr:uid="{D0FABE90-94BB-4510-8A04-3DED000903A4}">
       <formula1>F3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates some of the project metadata with info from mike s
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE92E5-2471-4A4C-9BB6-78FD5E5D6761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074016A4-C783-A447-8F80-6FCD7A07DC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t>first_name</t>
   </si>
@@ -201,9 +201,6 @@
     <t>principal investigator</t>
   </si>
   <si>
-    <t>Monitoring juvenile Chinook salmon outmigration using rotary screw traps on Battle and Clear Creek</t>
-  </si>
-  <si>
     <t>Battle and Clear RST</t>
   </si>
   <si>
@@ -246,7 +243,70 @@
     <t>chinook</t>
   </si>
   <si>
-    <t>Battle and Clear Rotary Screw Traps</t>
+    <t>Juvenile salmonid rotary screw trap data from Battle and Clear Creeks, Shasta and Tehama Counties, California.</t>
+  </si>
+  <si>
+    <t>Salmonid</t>
+  </si>
+  <si>
+    <t>Chinook</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>Passage</t>
+  </si>
+  <si>
+    <t>Catch</t>
+  </si>
+  <si>
+    <t>Oncorhynchus</t>
+  </si>
+  <si>
+    <t>tshawytscha</t>
+  </si>
+  <si>
+    <t>mykiss</t>
+  </si>
+  <si>
+    <t>Rotary screw trap</t>
+  </si>
+  <si>
+    <t>Winter-run</t>
+  </si>
+  <si>
+    <t>Spring-run</t>
+  </si>
+  <si>
+    <t>Fall-run</t>
+  </si>
+  <si>
+    <t>Late fall-run</t>
+  </si>
+  <si>
+    <t>Rainbow Trout</t>
+  </si>
+  <si>
+    <t>Steelhead</t>
+  </si>
+  <si>
+    <t>Clear Creek</t>
+  </si>
+  <si>
+    <t>Battle Creek</t>
+  </si>
+  <si>
+    <t>USBR</t>
+  </si>
+  <si>
+    <t>Battle Creek (Shasta and Tehama Cointies) and Clear Creek (Shasta Cointy) as one square</t>
+  </si>
+  <si>
+    <t>steelhead</t>
   </si>
 </sst>
 </file>
@@ -255,7 +315,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -326,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -346,9 +406,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -357,7 +414,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -743,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC88997-D746-4692-9A7F-1A0E218D4835}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +822,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
@@ -787,10 +844,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,7 +894,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +961,7 @@
       <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -907,16 +969,16 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -940,7 +1002,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -958,11 +1020,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -973,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,48 +1056,138 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>65</v>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1232,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1316,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,8 +1349,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
       <c r="D2" s="2"/>
@@ -1239,10 +1393,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1267,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="F10:G10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,26 +1458,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2">
-        <v>-122.49641099999999</v>
-      </c>
-      <c r="C2">
-        <v>-121.75038600000001</v>
+        <v>89</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-122.496668</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-122.14161199999999</v>
       </c>
       <c r="D2">
-        <v>40.505833330000002</v>
-      </c>
-      <c r="E2">
-        <v>39.622342000000003</v>
-      </c>
-      <c r="F2" s="16">
+        <v>40.506439</v>
+      </c>
+      <c r="E2" s="2">
+        <v>40.397897</v>
+      </c>
+      <c r="F2" s="15">
         <v>43831</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="15">
         <v>44928</v>
       </c>
     </row>
@@ -1343,12 +1497,12 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
builds edi package with methods
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074016A4-C783-A447-8F80-6FCD7A07DC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C41768A-F047-4C42-AD08-2EC1727EE9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>first_name</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Battle Creek</t>
-  </si>
-  <si>
-    <t>USBR</t>
   </si>
   <si>
     <t>Battle Creek (Shasta and Tehama Cointies) and Clear Creek (Shasta Cointy) as one square</t>
@@ -800,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC88997-D746-4692-9A7F-1A0E218D4835}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +896,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +915,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1250,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,21 +1281,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1316,7 +1301,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,10 +1334,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>88</v>
-      </c>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8"/>
       <c r="D2" s="2"/>
@@ -1460,7 +1443,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>-122.496668</v>

</xml_diff>

<commit_message>
updates coverage and project metadata, fixes latex issues in abstract and methods
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C41768A-F047-4C42-AD08-2EC1727EE9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE427C5-F25C-FD4A-80EB-5C54F8D7CB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -383,13 +383,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -412,6 +409,8 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -804,7 +803,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="7"/>
+    <col min="3" max="3" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -814,12 +813,12 @@
       <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
@@ -850,42 +849,42 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="21" style="7" customWidth="1"/>
-    <col min="4" max="8" width="10.5" style="7"/>
-    <col min="9" max="9" width="10.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21" style="6" customWidth="1"/>
+    <col min="4" max="8" width="10.5" style="6"/>
+    <col min="9" max="9" width="10.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -922,7 +921,7 @@
   <cols>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -941,7 +940,7 @@
       <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -958,7 +957,7 @@
       <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -966,16 +965,16 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1017,10 +1016,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1041,59 +1040,59 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1204,26 +1203,26 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="7"/>
-    <col min="4" max="4" width="15.1640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="26" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="6"/>
+    <col min="4" max="4" width="15.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1247,36 +1246,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="9" style="5"/>
-    <col min="4" max="4" width="9" style="7"/>
-    <col min="5" max="5" width="14.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9" style="5"/>
+    <col min="1" max="2" width="9" style="6"/>
+    <col min="3" max="3" width="9" style="4"/>
+    <col min="4" max="4" width="9" style="6"/>
+    <col min="5" max="5" width="14.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1307,40 +1306,40 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="5"/>
-    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="4"/>
+    <col min="6" max="6" width="17.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1363,14 +1362,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1378,7 +1377,7 @@
       <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1404,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,8 +1440,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="2">
@@ -1457,35 +1456,35 @@
       <c r="E2" s="2">
         <v>40.397897</v>
       </c>
-      <c r="F2" s="15">
-        <v>43831</v>
-      </c>
-      <c r="G2" s="15">
+      <c r="F2" s="14">
+        <v>36039</v>
+      </c>
+      <c r="G2" s="14">
         <v>44928</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" s="4"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" s="4"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="4"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
updates time coverage and makes mike contact in project metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE427C5-F25C-FD4A-80EB-5C54F8D7CB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41415FD-13FF-7143-8F80-3D4D0689520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -383,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -409,8 +409,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -913,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,7 +954,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>50</v>
@@ -972,7 +971,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>50</v>
@@ -1016,7 +1015,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1403,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1440,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="2">
@@ -1460,7 +1459,7 @@
         <v>36039</v>
       </c>
       <c r="G2" s="14">
-        <v>44928</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updates project maintenance field
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41415FD-13FF-7143-8F80-3D4D0689520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95548337-73CB-E04A-8118-D21E138EE1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t xml:space="preserve">ongoing </t>
   </si>
   <si>
-    <t>monthly</t>
-  </si>
-  <si>
     <t>chinook</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>steelhead</t>
+  </si>
+  <si>
+    <t>annually</t>
   </si>
 </sst>
 </file>
@@ -889,12 +889,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>55</v>
@@ -1097,92 +1097,92 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,7 +1377,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2">
         <v>-122.496668</v>

</xml_diff>

<commit_message>
updates with new data from natasha
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata.xlsx
+++ b/data-raw/metadata/project-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3456A390-CB45-0449-9F0E-60AE05578EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBABEE32-DBCC-544A-8CA6-A540A779642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35120" yWindow="1680" windowWidth="28800" windowHeight="16540" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>first_name</t>
   </si>
@@ -187,18 +187,6 @@
   </si>
   <si>
     <t>U.S. Fish and Wildlife Service</t>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schraml </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mike_schraml@fws.gov </t>
-  </si>
-  <si>
-    <t>principal investigator</t>
   </si>
   <si>
     <t>Battle and Clear RST</t>
@@ -320,7 +308,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -347,12 +335,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -389,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -407,8 +389,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -895,12 +875,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -916,10 +896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,39 +940,19 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1005" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1004" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="mailto:mike_schraml@fws.gov" xr:uid="{F2D40BA9-AE88-344B-8932-8A4AF3E71FFF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1022,10 +982,10 @@
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1058,147 +1018,147 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1243,7 +1203,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1390,10 +1350,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1379,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1456,8 +1416,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>87</v>
+      <c r="A2" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="B2" s="2">
         <v>-122.496668</v>
@@ -1471,11 +1431,11 @@
       <c r="E2" s="2">
         <v>40.397897</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <v>36039</v>
       </c>
-      <c r="G2" s="14">
-        <v>45749</v>
+      <c r="G2" s="12">
+        <v>45847</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1494,12 +1454,12 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>